<commit_message>
gan xog toa thuoc
</commit_message>
<xml_diff>
--- a/Prj2/save/QLTuThuoc.xlsx
+++ b/Prj2/save/QLTuThuoc.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TuThuoc-SceneBuilder\Medicine\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C866016-6D91-4137-9DF6-AEEB1C838247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9C866016-6D91-4137-9DF6-AEEB1C838247}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="16440" windowWidth="29040" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="MEDICINE" sheetId="1" r:id="rId1"/>
-    <sheet name="PRESCRIPTION" sheetId="2" r:id="rId2"/>
-    <sheet name="DISEASE" sheetId="3" r:id="rId3"/>
-    <sheet name="MEDICINE-PRESCRIPTION" sheetId="4" r:id="rId4"/>
-    <sheet name="INSTRUMENT" sheetId="5" r:id="rId5"/>
+    <sheet name="MEDICINE" r:id="rId1" sheetId="1"/>
+    <sheet name="PRESCRIPTION" r:id="rId2" sheetId="2"/>
+    <sheet name="DISEASE" r:id="rId3" sheetId="3"/>
+    <sheet name="MEDICINE-PRESCRIPTION" r:id="rId4" sheetId="4"/>
+    <sheet name="INSTRUMENT" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,18 @@
   <si>
     <t>Dung sat trung vet thuong</t>
   </si>
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
 </sst>
 </file>
 
@@ -266,32 +278,44 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="19">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -415,21 +439,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -446,7 +470,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -500,20 +524,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="8" max="8" width="107" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="107.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
@@ -560,473 +584,236 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="C2" t="n">
+        <v>2.0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
-        <v>45005</v>
+      <c r="F2" t="n" s="18">
+        <v>45005.0</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
+      <c r="H2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
-        <v>5</v>
+      <c r="C3" t="n">
+        <v>5.0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3">
-        <v>44757</v>
+      <c r="F3" t="n" s="18">
+        <v>44757.0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
+      <c r="H3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
+      <c r="C4" t="n">
+        <v>1.0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3">
-        <v>45000</v>
+      <c r="F4" t="n" s="18">
+        <v>45000.0</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
+      <c r="H4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
+      <c r="C5" t="n">
+        <v>1.0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3">
-        <v>45119</v>
+      <c r="F5" t="n" s="18">
+        <v>45119.0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
+      <c r="H5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1">
-        <v>3</v>
+      <c r="C6" t="n">
+        <v>3.0</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3">
-        <v>44757</v>
+      <c r="F6" t="n" s="18">
+        <v>44757.0</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
+      <c r="H6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1">
-        <v>5</v>
+      <c r="C7" t="n">
+        <v>5.0</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="3">
-        <v>37467</v>
+      <c r="F7" t="n" s="18">
+        <v>37467.0</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
+      <c r="H7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1">
-        <v>2</v>
+      <c r="C8" t="n">
+        <v>2.0</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="3">
-        <v>37467</v>
+      <c r="F8" t="n" s="18">
+        <v>37467.0</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
+      <c r="H8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1">
-        <v>4</v>
+      <c r="C9" t="n">
+        <v>4.0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3">
-        <v>45000</v>
+      <c r="F9" t="n" s="18">
+        <v>45000.0</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
+      <c r="H9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>35</v>
+      <c r="B10" t="s">
+        <v>36</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="C10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>36</v>
+      <c r="E10" t="s">
+        <v>37</v>
       </c>
-      <c r="C10" s="1">
-        <v>2</v>
+      <c r="F10" t="n" s="18">
+        <v>37467.0</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="H10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="3">
-        <v>37467</v>
+      <c r="F11" t="n" s="18">
+        <v>45005.0</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>16</v>
+      <c r="H11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>38</v>
+      <c r="B12" t="s">
+        <v>65</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="C12" t="n">
+        <v>1.0</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
+      <c r="D12" t="s">
+        <v>66</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
+      <c r="E12" t="s">
+        <v>66</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
+      <c r="F12" t="n" s="18">
+        <v>44741.0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="3">
-        <v>45005</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
+      <c r="H12"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -28694,32 +28481,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink r:id="rId1" ref="H2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="H3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId3" ref="H4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink r:id="rId4" ref="H5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink r:id="rId5" ref="H6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink r:id="rId6" ref="H7" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink r:id="rId7" ref="H8" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink r:id="rId8" ref="H9" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink r:id="rId9" ref="H10" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink r:id="rId10" ref="H11" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId11"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId11" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -28744,20 +28531,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
@@ -28808,20 +28595,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
@@ -28848,20 +28635,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -28901,279 +28688,141 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="C2" t="n">
+        <v>2.0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="E2" t="s">
+        <v>55</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
+      <c r="C3" t="n">
+        <v>1.0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="E3" t="s">
+        <v>55</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
+      <c r="C4" t="n">
+        <v>1.0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="E4" t="s">
+        <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="1">
-        <v>2</v>
+      <c r="C5" t="n">
+        <v>2.0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="E5" t="s">
+        <v>60</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="1">
-        <v>2</v>
+      <c r="C6" t="n">
+        <v>2.0</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -56924,6 +56573,6 @@
       <c r="Z1000" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cap nhat tam thoi
</commit_message>
<xml_diff>
--- a/Prj2/save/QLTuThuoc.xlsx
+++ b/Prj2/save/QLTuThuoc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -219,6 +219,15 @@
   </si>
   <si>
     <t>Điều trị táo bón</t>
+  </si>
+  <si>
+    <t>phuc</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -262,13 +271,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -556,7 +573,7 @@
       <c r="E2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="n" s="17">
+      <c r="F2" t="n" s="25">
         <v>44757.0</v>
       </c>
       <c r="H2"/>
@@ -577,7 +594,7 @@
       <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" t="n" s="17">
+      <c r="F3" t="n" s="25">
         <v>45000.0</v>
       </c>
       <c r="H3"/>
@@ -598,7 +615,7 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" t="n" s="17">
+      <c r="F4" t="n" s="25">
         <v>45119.0</v>
       </c>
       <c r="H4"/>
@@ -619,7 +636,7 @@
       <c r="E5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" t="n" s="17">
+      <c r="F5" t="n" s="25">
         <v>44757.0</v>
       </c>
       <c r="H5"/>
@@ -640,7 +657,7 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="n" s="17">
+      <c r="F6" t="n" s="25">
         <v>37467.0</v>
       </c>
       <c r="H6"/>
@@ -661,7 +678,7 @@
       <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="n" s="17">
+      <c r="F7" t="n" s="25">
         <v>37467.0</v>
       </c>
       <c r="H7"/>
@@ -682,7 +699,7 @@
       <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="n" s="17">
+      <c r="F8" t="n" s="25">
         <v>37467.0</v>
       </c>
       <c r="H8"/>
@@ -703,7 +720,7 @@
       <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="n" s="17">
+      <c r="F9" t="n" s="25">
         <v>45005.0</v>
       </c>
       <c r="H9"/>
@@ -724,29 +741,29 @@
       <c r="E10" t="s">
         <v>54</v>
       </c>
-      <c r="F10" t="n" s="17">
+      <c r="F10" t="n" s="25">
         <v>44772.0</v>
       </c>
       <c r="H10"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C11" t="n">
-        <v>123.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" t="n" s="17">
-        <v>44746.0</v>
+        <v>67</v>
+      </c>
+      <c r="F11" t="n" s="25">
+        <v>44752.0</v>
       </c>
       <c r="H11"/>
     </row>

</xml_diff>